<commit_message>
Fixed a mistake in a label
</commit_message>
<xml_diff>
--- a/PreventableDeaths.xlsx
+++ b/PreventableDeaths.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>Preventable COVID-19 Deaths, with available vaccination, 4/15/21 to 7/15/21</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>Vaccinated at start</t>
+  </si>
+  <si>
+    <t>Vaccinated at end</t>
   </si>
   <si>
     <t>US adult population</t>
@@ -1932,7 +1935,7 @@
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" t="s" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" s="15">
         <v>167000000</v>
@@ -1950,7 +1953,7 @@
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" t="s" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" s="15">
         <v>260000000</v>
@@ -1961,7 +1964,7 @@
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" t="s" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B11" s="17">
         <f>B10-B8</f>
@@ -1973,7 +1976,7 @@
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" t="s" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B12" s="17">
         <f>B11/2</f>
@@ -1992,7 +1995,7 @@
     </row>
     <row r="14" ht="20.05" customHeight="1">
       <c r="A14" t="s" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B14" s="18">
         <v>3.86</v>
@@ -2003,7 +2006,7 @@
     </row>
     <row r="15" ht="20.05" customHeight="1">
       <c r="A15" t="s" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B15" s="18">
         <v>0.24</v>
@@ -2021,7 +2024,7 @@
     </row>
     <row r="17" ht="20.05" customHeight="1">
       <c r="A17" t="s" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B17" s="17">
         <f>B12/100000*12*B14</f>
@@ -2033,7 +2036,7 @@
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" t="s" s="7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B18" s="17">
         <f>B12/100000*12*B15</f>
@@ -2045,7 +2048,7 @@
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" t="s" s="7">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B19" s="19">
         <f>B17-B18</f>
@@ -2064,7 +2067,7 @@
     </row>
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" t="s" s="20">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="9"/>
@@ -2074,7 +2077,7 @@
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" s="13"/>
       <c r="B22" t="s" s="21">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -2083,7 +2086,7 @@
     <row r="23" ht="20.05" customHeight="1">
       <c r="A23" s="13"/>
       <c r="B23" t="s" s="21">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -2121,7 +2124,7 @@
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2131,22 +2134,22 @@
     </row>
     <row r="2" ht="44.25" customHeight="1">
       <c r="A2" t="s" s="23">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s" s="23">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s" s="23">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s" s="23">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s" s="23">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s" s="23">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" ht="20.25" customHeight="1">
@@ -2305,7 +2308,7 @@
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" t="s" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="32"/>
       <c r="C10" s="33"/>
@@ -2332,7 +2335,7 @@
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" s="15">
         <v>313000000</v>
@@ -2344,7 +2347,7 @@
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B13" s="15">
         <v>332000000</v>
@@ -2401,7 +2404,7 @@
     </row>
     <row r="18" ht="32.05" customHeight="1">
       <c r="A18" t="s" s="7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B18" s="17">
         <f>B12/100000*(52+10)*F10</f>
@@ -2414,7 +2417,7 @@
     </row>
     <row r="19" ht="32.05" customHeight="1">
       <c r="A19" t="s" s="39">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B19" s="40">
         <f>B17-B18</f>
@@ -2435,7 +2438,7 @@
     </row>
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" t="s" s="44">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21" s="45"/>
       <c r="C21" s="9"/>
@@ -2445,10 +2448,10 @@
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" t="s" s="7">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s" s="21">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -2457,10 +2460,10 @@
     </row>
     <row r="23" ht="20.05" customHeight="1">
       <c r="A23" t="s" s="7">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s" s="21">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -2469,10 +2472,10 @@
     </row>
     <row r="24" ht="20.05" customHeight="1">
       <c r="A24" t="s" s="7">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s" s="21">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -2481,10 +2484,10 @@
     </row>
     <row r="25" ht="20.05" customHeight="1">
       <c r="A25" t="s" s="7">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s" s="21">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -2493,10 +2496,10 @@
     </row>
     <row r="26" ht="20.05" customHeight="1">
       <c r="A26" t="s" s="7">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s" s="46">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
@@ -2513,7 +2516,7 @@
     </row>
     <row r="28" ht="20.05" customHeight="1">
       <c r="A28" t="s" s="20">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="9"/>
@@ -2524,7 +2527,7 @@
     <row r="29" ht="20.05" customHeight="1">
       <c r="A29" s="13"/>
       <c r="B29" t="s" s="21">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
@@ -2534,7 +2537,7 @@
     <row r="30" ht="20.05" customHeight="1">
       <c r="A30" s="13"/>
       <c r="B30" t="s" s="21">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -2544,7 +2547,7 @@
     <row r="31" ht="20.05" customHeight="1">
       <c r="A31" s="13"/>
       <c r="B31" t="s" s="21">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
@@ -2554,7 +2557,7 @@
     <row r="32" ht="20.05" customHeight="1">
       <c r="A32" s="13"/>
       <c r="B32" t="s" s="21">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -2564,7 +2567,7 @@
     <row r="33" ht="20.05" customHeight="1">
       <c r="A33" s="13"/>
       <c r="B33" t="s" s="21">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
@@ -2574,7 +2577,7 @@
     <row r="34" ht="20.05" customHeight="1">
       <c r="A34" s="13"/>
       <c r="B34" t="s" s="21">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -2899,7 +2902,7 @@
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2956,7 +2959,7 @@
     </row>
     <row r="7" ht="32.05" customHeight="1">
       <c r="A7" t="s" s="52">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B7" s="51">
         <f>'April 21 - July 21'!B19</f>
@@ -2968,7 +2971,7 @@
     </row>
     <row r="8" ht="32.05" customHeight="1">
       <c r="A8" t="s" s="52">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B8" s="51">
         <f>'July 21 - Sept 22'!B19</f>
@@ -2980,7 +2983,7 @@
     </row>
     <row r="9" ht="32.05" customHeight="1">
       <c r="A9" t="s" s="53">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="54">
         <f>B7+B8</f>
@@ -2999,7 +3002,7 @@
     </row>
     <row r="11" ht="32.05" customHeight="1">
       <c r="A11" t="s" s="7">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B11" s="55">
         <f>B9/B5</f>

</xml_diff>

<commit_message>
Updated with today's data
</commit_message>
<xml_diff>
--- a/PreventableDeaths.xlsx
+++ b/PreventableDeaths.xlsx
@@ -6,8 +6,8 @@
   </bookViews>
   <sheets>
     <sheet name="April 21 - July 21" sheetId="1" r:id="rId4"/>
-    <sheet name="July 21 - Sept 22" sheetId="2" r:id="rId5"/>
-    <sheet name="April 21 - Sept 22" sheetId="3" r:id="rId6"/>
+    <sheet name="July 21 - Dec 22" sheetId="2" r:id="rId5"/>
+    <sheet name="April 21 - Dec 22" sheetId="3" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -66,7 +66,7 @@
     <t>Vaccinated = completed primary series (usually 2 shots)</t>
   </si>
   <si>
-    <t>Preventable COVID-19 Deaths, with available vaccination, 7/15/21 to 9/25/22</t>
+    <t>Preventable COVID-19 Deaths, with available vaccination, 7/15/21 to 12/14/22</t>
   </si>
   <si>
     <t>Date</t>
@@ -182,7 +182,7 @@
     </r>
   </si>
   <si>
-    <t>Vaccinated = primary series + 1 or more boosters as recommended.</t>
+    <t>Vaccinated = primary series + all boosters recommended.</t>
   </si>
   <si>
     <t>Unvaxed death rates are out of the total unvaccinated population.</t>
@@ -197,13 +197,13 @@
     <t>Unvaxed deaths for 7/21 and 9/21 use a population base of 6+ months. This does not affect any key calculations here.</t>
   </si>
   <si>
-    <t>Preventable COVID-19 Deaths, with available vaccination, 4/15/21 to 9/25/22</t>
+    <t>Preventable COVID-19 Deaths, with available vaccination, 4/15/21 to 12/14/22</t>
   </si>
   <si>
     <t>Preventable deaths 4/15/21 to 7/15/21, estimated</t>
   </si>
   <si>
-    <t>Preventable deaths 7/15/21 to 9/25/22, estimated</t>
+    <t>Preventable deaths 7/15/21 to 12/14/22, estimated</t>
   </si>
   <si>
     <t>Preventable deaths fraction of actual deaths, estimated</t>
@@ -2106,7 +2106,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:F69"/>
+  <dimension ref="A2:F70"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -2166,12 +2166,12 @@
         <v>276</v>
       </c>
       <c r="E3" s="27">
-        <f>D3/D10</f>
-        <v>0.0400696864111498</v>
+        <f>D3/D11</f>
+        <v>0.0380584666298952</v>
       </c>
       <c r="F3" s="27">
         <f>C3*E3</f>
-        <v>0.0196341463414634</v>
+        <v>0.0186486486486486</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
@@ -2188,12 +2188,12 @@
         <v>1716</v>
       </c>
       <c r="E4" s="31">
-        <f>D4/D10</f>
-        <v>0.249128919860627</v>
+        <f>D4/D11</f>
+        <v>0.236624379481522</v>
       </c>
       <c r="F4" s="31">
         <f>C4*E4</f>
-        <v>0.246637630662021</v>
+        <v>0.234258135686707</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
@@ -2210,12 +2210,12 @@
         <v>1028</v>
       </c>
       <c r="E5" s="31">
-        <f>D5/D10</f>
-        <v>0.14924506387921</v>
+        <f>D5/D11</f>
+        <v>0.141753998896856</v>
       </c>
       <c r="F5" s="31">
         <f>C5*E5</f>
-        <v>0.0358188153310104</v>
+        <v>0.0340209597352454</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
@@ -2232,12 +2232,12 @@
         <v>1934</v>
       </c>
       <c r="E6" s="31">
-        <f>D6/D10</f>
-        <v>0.280778164924506</v>
+        <f>D6/D11</f>
+        <v>0.266685052399338</v>
       </c>
       <c r="F6" s="31">
         <f>C6*E6</f>
-        <v>0.381858304297328</v>
+        <v>0.3626916712631</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
@@ -2254,12 +2254,12 @@
         <v>1234</v>
       </c>
       <c r="E7" s="31">
-        <f>D7/D10</f>
-        <v>0.179152148664344</v>
+        <f>D7/D11</f>
+        <v>0.170159955874242</v>
       </c>
       <c r="F7" s="31">
         <f>C7*E7</f>
-        <v>0.0197067363530778</v>
+        <v>0.0187175951461666</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
@@ -2276,12 +2276,12 @@
         <v>288</v>
       </c>
       <c r="E8" s="31">
-        <f>D8/D10</f>
-        <v>0.0418118466898955</v>
+        <f>D8/D11</f>
+        <v>0.0397131825703254</v>
       </c>
       <c r="F8" s="31">
         <f>C8*E8</f>
-        <v>0.0121254355400697</v>
+        <v>0.0115168229453944</v>
       </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
@@ -2298,48 +2298,58 @@
         <v>412</v>
       </c>
       <c r="E9" s="31">
-        <f>D9/D10</f>
-        <v>0.0598141695702671</v>
+        <f>D9/D11</f>
+        <v>0.0568119139547711</v>
       </c>
       <c r="F9" s="31">
         <f>C9*E9</f>
-        <v>0.0239256678281068</v>
+        <v>0.0227247655819084</v>
       </c>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="7">
+      <c r="A10" s="28">
+        <v>44857</v>
+      </c>
+      <c r="B10" s="29">
+        <v>1.17</v>
+      </c>
+      <c r="C10" s="30">
+        <v>0.04</v>
+      </c>
+      <c r="D10" s="30">
+        <v>364</v>
+      </c>
+      <c r="E10" s="31">
+        <f>D10/D11</f>
+        <v>0.0501930501930502</v>
+      </c>
+      <c r="F10" s="31">
+        <f>C10*E10</f>
+        <v>0.00200772200772201</v>
+      </c>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" t="s" s="7">
         <v>24</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="34">
-        <f>SUM(D3:D9)</f>
-        <v>6888</v>
-      </c>
-      <c r="E10" s="35">
-        <f>SUM(E3:E9)</f>
-        <v>0.999999999999999</v>
-      </c>
-      <c r="F10" s="36">
-        <f>SUM(F3:F9)</f>
-        <v>0.739706736353077</v>
-      </c>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="13"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="34">
+        <f>SUM(D3:D10)</f>
+        <v>7252</v>
+      </c>
+      <c r="E11" s="35">
+        <f>SUM(E3:E10)</f>
+        <v>1</v>
+      </c>
+      <c r="F11" s="36">
+        <f>SUM(F3:F10)</f>
+        <v>0.704586321014892</v>
+      </c>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="7">
-        <v>25</v>
-      </c>
-      <c r="B12" s="15">
-        <v>313000000</v>
-      </c>
+      <c r="A12" s="13"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -2347,10 +2357,10 @@
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" t="s" s="7">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="15">
-        <v>332000000</v>
+        <v>313000000</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -2358,31 +2368,31 @@
       <c r="F13" s="9"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="13"/>
-      <c r="B14" s="16"/>
+      <c r="A14" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="B14" s="15">
+        <v>332000000</v>
+      </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
     </row>
-    <row r="15" ht="22.35" customHeight="1">
-      <c r="A15" t="s" s="7">
-        <v>1</v>
-      </c>
-      <c r="B15" s="37">
-        <v>607834</v>
-      </c>
+    <row r="15" ht="20.05" customHeight="1">
+      <c r="A15" s="13"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="38"/>
+      <c r="E15" s="9"/>
       <c r="F15" s="9"/>
     </row>
     <row r="16" ht="22.35" customHeight="1">
       <c r="A16" t="s" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" s="37">
-        <v>1051501</v>
+        <v>607834</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
@@ -2391,68 +2401,68 @@
     </row>
     <row r="17" ht="22.35" customHeight="1">
       <c r="A17" t="s" s="7">
-        <v>3</v>
-      </c>
-      <c r="B17" s="17">
-        <f>B16-B15</f>
-        <v>443667</v>
+        <v>2</v>
+      </c>
+      <c r="B17" s="37">
+        <v>1083279</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="38"/>
       <c r="F17" s="9"/>
     </row>
-    <row r="18" ht="32.05" customHeight="1">
+    <row r="18" ht="22.35" customHeight="1">
       <c r="A18" t="s" s="7">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="B18" s="17">
-        <f>B12/100000*(52+10)*F10</f>
-        <v>143547.489256678</v>
+        <f>B17-B16</f>
+        <v>475445</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
+      <c r="E18" s="38"/>
       <c r="F18" s="9"/>
     </row>
     <row r="19" ht="32.05" customHeight="1">
-      <c r="A19" t="s" s="39">
-        <v>13</v>
-      </c>
-      <c r="B19" s="40">
-        <f>B17-B18</f>
-        <v>300119.510743322</v>
+      <c r="A19" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="B19" s="17">
+        <f>B13/100000*(52+10)*F11</f>
+        <v>136732.02145615</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
     </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="41"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="43"/>
+    <row r="20" ht="32.05" customHeight="1">
+      <c r="A20" t="s" s="39">
+        <v>13</v>
+      </c>
+      <c r="B20" s="40">
+        <f>B18-B19</f>
+        <v>338712.97854385</v>
+      </c>
+      <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" t="s" s="44">
-        <v>28</v>
-      </c>
-      <c r="B21" s="45"/>
-      <c r="C21" s="9"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="43"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="B22" t="s" s="21">
-        <v>30</v>
-      </c>
+      <c r="A22" t="s" s="44">
+        <v>28</v>
+      </c>
+      <c r="B22" s="45"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -2460,10 +2470,10 @@
     </row>
     <row r="23" ht="20.05" customHeight="1">
       <c r="A23" t="s" s="7">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s" s="21">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -2472,10 +2482,10 @@
     </row>
     <row r="24" ht="20.05" customHeight="1">
       <c r="A24" t="s" s="7">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s" s="21">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -2484,10 +2494,10 @@
     </row>
     <row r="25" ht="20.05" customHeight="1">
       <c r="A25" t="s" s="7">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s" s="21">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -2496,10 +2506,10 @@
     </row>
     <row r="26" ht="20.05" customHeight="1">
       <c r="A26" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="B26" t="s" s="46">
-        <v>38</v>
+        <v>35</v>
+      </c>
+      <c r="B26" t="s" s="21">
+        <v>36</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
@@ -2507,17 +2517,19 @@
       <c r="F26" s="9"/>
     </row>
     <row r="27" ht="20.05" customHeight="1">
-      <c r="A27" s="47"/>
-      <c r="B27" s="16"/>
+      <c r="A27" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="B27" t="s" s="46">
+        <v>38</v>
+      </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
     </row>
     <row r="28" ht="20.05" customHeight="1">
-      <c r="A28" t="s" s="20">
-        <v>14</v>
-      </c>
+      <c r="A28" s="47"/>
       <c r="B28" s="16"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -2525,10 +2537,10 @@
       <c r="F28" s="9"/>
     </row>
     <row r="29" ht="20.05" customHeight="1">
-      <c r="A29" s="13"/>
-      <c r="B29" t="s" s="21">
-        <v>39</v>
-      </c>
+      <c r="A29" t="s" s="20">
+        <v>14</v>
+      </c>
+      <c r="B29" s="16"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
@@ -2537,7 +2549,7 @@
     <row r="30" ht="20.05" customHeight="1">
       <c r="A30" s="13"/>
       <c r="B30" t="s" s="21">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -2547,7 +2559,7 @@
     <row r="31" ht="20.05" customHeight="1">
       <c r="A31" s="13"/>
       <c r="B31" t="s" s="21">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
@@ -2557,7 +2569,7 @@
     <row r="32" ht="20.05" customHeight="1">
       <c r="A32" s="13"/>
       <c r="B32" t="s" s="21">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -2567,7 +2579,7 @@
     <row r="33" ht="20.05" customHeight="1">
       <c r="A33" s="13"/>
       <c r="B33" t="s" s="21">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
@@ -2577,7 +2589,7 @@
     <row r="34" ht="20.05" customHeight="1">
       <c r="A34" s="13"/>
       <c r="B34" t="s" s="21">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -2586,7 +2598,9 @@
     </row>
     <row r="35" ht="20.05" customHeight="1">
       <c r="A35" s="13"/>
-      <c r="B35" s="16"/>
+      <c r="B35" t="s" s="21">
+        <v>44</v>
+      </c>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
@@ -2594,7 +2608,7 @@
     </row>
     <row r="36" ht="20.05" customHeight="1">
       <c r="A36" s="13"/>
-      <c r="B36" s="48"/>
+      <c r="B36" s="16"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
@@ -2864,15 +2878,23 @@
       <c r="E69" s="9"/>
       <c r="F69" s="9"/>
     </row>
+    <row r="70" ht="20.05" customHeight="1">
+      <c r="A70" s="13"/>
+      <c r="B70" s="48"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B22" r:id="rId1" location="" tooltip="" display="https://covid.cdc.gov/covid-data-tracker/#trends_dailydeaths_select_00"/>
-    <hyperlink ref="B23" r:id="rId2" location="" tooltip="" display="https://covid.cdc.gov/covid-data-tracker/#rates-by-vaccine-status"/>
-    <hyperlink ref="B24" r:id="rId3" location="" tooltip="" display="https://covid.cdc.gov/covid-data-tracker/#vaccination-trends"/>
-    <hyperlink ref="B25" r:id="rId4" location="" tooltip="" display="https://covid.cdc.gov/covid-data-tracker/#vaccination-demographics-trends"/>
+    <hyperlink ref="B23" r:id="rId1" location="" tooltip="" display="https://covid.cdc.gov/covid-data-tracker/#trends_dailydeaths_select_00"/>
+    <hyperlink ref="B24" r:id="rId2" location="" tooltip="" display="https://covid.cdc.gov/covid-data-tracker/#rates-by-vaccine-status"/>
+    <hyperlink ref="B25" r:id="rId3" location="" tooltip="" display="https://covid.cdc.gov/covid-data-tracker/#vaccination-trends"/>
+    <hyperlink ref="B26" r:id="rId4" location="" tooltip="" display="https://covid.cdc.gov/covid-data-tracker/#vaccination-demographics-trends"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -2932,7 +2954,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="37">
-        <v>1051501</v>
+        <v>1083279</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -2944,7 +2966,7 @@
       </c>
       <c r="B5" s="50">
         <f>B4-B3</f>
-        <v>484501</v>
+        <v>516279</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -2974,8 +2996,8 @@
         <v>47</v>
       </c>
       <c r="B8" s="51">
-        <f>'July 21 - Sept 22'!B19</f>
-        <v>300119.510743322</v>
+        <f>'July 21 - Dec 22'!B20</f>
+        <v>338712.97854385</v>
       </c>
       <c r="C8" s="43"/>
       <c r="D8" s="9"/>
@@ -2987,7 +3009,7 @@
       </c>
       <c r="B9" s="54">
         <f>B7+B8</f>
-        <v>320319.110743322</v>
+        <v>358912.57854385</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -3006,7 +3028,7 @@
       </c>
       <c r="B11" s="55">
         <f>B9/B5</f>
-        <v>0.66113199094186</v>
+        <v>0.695191124457609</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>

</xml_diff>